<commit_message>
Update inventory management Excel with alerts and dashboard enhancements
</commit_message>
<xml_diff>
--- a/Inventory_Management.xlsx
+++ b/Inventory_Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0b71cfb104e05f34/Documents/EXCEL SHEETS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="566" documentId="8_{EE203A3D-4A42-4892-9665-C5DF87507929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0B2B308-1E9A-4471-8C52-8CCF7167C381}"/>
+  <xr:revisionPtr revIDLastSave="587" documentId="8_{EE203A3D-4A42-4892-9665-C5DF87507929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5ACAD6EA-A9A3-47B5-9873-7C9673F717F4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{032C2DBF-5864-48A2-A9A8-6779FA321EC7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="70">
   <si>
     <t>Product_ID</t>
   </si>
@@ -238,6 +238,15 @@
   </si>
   <si>
     <t>Healthy Stock</t>
+  </si>
+  <si>
+    <t>Last_Updated</t>
+  </si>
+  <si>
+    <t>Reorder_Quantity</t>
+  </si>
+  <si>
+    <t>Products Needing Action</t>
   </si>
 </sst>
 </file>
@@ -414,7 +423,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-IN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2405,14 +2414,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>168346</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>68286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>21687</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>178018</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>77957</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2440,15 +2449,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>70555</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>151000</xdr:rowOff>
+      <xdr:colOff>47464</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>58637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>169875</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>176389</xdr:rowOff>
+      <xdr:colOff>146784</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>84025</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4663,10 +4672,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6C1311-957A-47ED-B2E7-19F5194E02C2}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="E21" sqref="A1:E21"/>
+      <selection activeCell="G2" sqref="G2:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4676,9 +4685,11 @@
     <col min="3" max="3" width="15.77734375" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="11.21875" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4694,8 +4705,14 @@
       <c r="E1" s="8" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
@@ -4719,8 +4736,16 @@
         <f>IF(C2&lt;0,"DATA ISSUE",IF(C2&lt;=D2,"LOW STOCK","OK"))</f>
         <v>OK</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <f>_xlfn.MAXIFS(Stock_Movements!A:A,Stock_Movements!B:B,A2)</f>
+        <v>46011</v>
+      </c>
+      <c r="G2" t="str">
+        <f>IF(C2&lt;=D2,(D2*2)-C2,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -4744,8 +4769,16 @@
         <f t="shared" ref="E3:E21" si="0">IF(C3&lt;0,"DATA ISSUE",IF(C3&lt;=D3,"LOW STOCK","OK"))</f>
         <v>LOW STOCK</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <f>_xlfn.MAXIFS(Stock_Movements!A:A,Stock_Movements!B:B,A3)</f>
+        <v>46012</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G21" si="1">IF(C3&lt;=D3,(D3*2)-C3,"")</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -4769,8 +4802,16 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <f>_xlfn.MAXIFS(Stock_Movements!A:A,Stock_Movements!B:B,A4)</f>
+        <v>46013</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -4794,8 +4835,16 @@
         <f t="shared" si="0"/>
         <v>LOW STOCK</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <f>_xlfn.MAXIFS(Stock_Movements!A:A,Stock_Movements!B:B,A5)</f>
+        <v>46014</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -4819,8 +4868,16 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <f>_xlfn.MAXIFS(Stock_Movements!A:A,Stock_Movements!B:B,A6)</f>
+        <v>46015</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -4844,8 +4901,16 @@
         <f t="shared" si="0"/>
         <v>LOW STOCK</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <f>_xlfn.MAXIFS(Stock_Movements!A:A,Stock_Movements!B:B,A7)</f>
+        <v>46016</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -4869,8 +4934,16 @@
         <f t="shared" si="0"/>
         <v>DATA ISSUE</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <f>_xlfn.MAXIFS(Stock_Movements!A:A,Stock_Movements!B:B,A8)</f>
+        <v>46017</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -4894,8 +4967,16 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <f>_xlfn.MAXIFS(Stock_Movements!A:A,Stock_Movements!B:B,A9)</f>
+        <v>46018</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>14</v>
       </c>
@@ -4919,8 +5000,16 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <f>_xlfn.MAXIFS(Stock_Movements!A:A,Stock_Movements!B:B,A10)</f>
+        <v>46019</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
@@ -4944,8 +5033,16 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <f>_xlfn.MAXIFS(Stock_Movements!A:A,Stock_Movements!B:B,A11)</f>
+        <v>46020</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
@@ -4969,8 +5066,16 @@
         <f t="shared" si="0"/>
         <v>DATA ISSUE</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <f>_xlfn.MAXIFS(Stock_Movements!A:A,Stock_Movements!B:B,A12)</f>
+        <v>46021</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -4994,8 +5099,16 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <f>_xlfn.MAXIFS(Stock_Movements!A:A,Stock_Movements!B:B,A13)</f>
+        <v>46022</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>18</v>
       </c>
@@ -5019,8 +5132,16 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <f>_xlfn.MAXIFS(Stock_Movements!A:A,Stock_Movements!B:B,A14)</f>
+        <v>46023</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
@@ -5044,8 +5165,16 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <f>_xlfn.MAXIFS(Stock_Movements!A:A,Stock_Movements!B:B,A15)</f>
+        <v>46024</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>20</v>
       </c>
@@ -5069,8 +5198,16 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <f>_xlfn.MAXIFS(Stock_Movements!A:A,Stock_Movements!B:B,A16)</f>
+        <v>46025</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>21</v>
       </c>
@@ -5094,8 +5231,16 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <f>_xlfn.MAXIFS(Stock_Movements!A:A,Stock_Movements!B:B,A17)</f>
+        <v>46026</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>22</v>
       </c>
@@ -5119,8 +5264,16 @@
         <f t="shared" si="0"/>
         <v>LOW STOCK</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <f>_xlfn.MAXIFS(Stock_Movements!A:A,Stock_Movements!B:B,A18)</f>
+        <v>46027</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>23</v>
       </c>
@@ -5144,8 +5297,16 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <f>_xlfn.MAXIFS(Stock_Movements!A:A,Stock_Movements!B:B,A19)</f>
+        <v>46028</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>24</v>
       </c>
@@ -5169,8 +5330,16 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <f>_xlfn.MAXIFS(Stock_Movements!A:A,Stock_Movements!B:B,A20)</f>
+        <v>46029</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>25</v>
       </c>
@@ -5193,6 +5362,14 @@
       <c r="E21" s="7" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
+      </c>
+      <c r="F21">
+        <f>_xlfn.MAXIFS(Stock_Movements!A:A,Stock_Movements!B:B,A21)</f>
+        <v>46030</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -5217,7 +5394,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5226,6 +5403,7 @@
     <col min="2" max="2" width="18.44140625" customWidth="1"/>
     <col min="3" max="3" width="19.44140625" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -5241,7 +5419,9 @@
       <c r="D1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="5"/>
+      <c r="E1" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
@@ -5260,7 +5440,11 @@
         <f>COUNTIF(Inventory_Status!E2:E21,"OK")</f>
         <v>14</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="E2" s="5">
+        <f>COUNTIF(Inventory_Status!E:E,"DATA ISSUE")
+ + COUNTIF(Inventory_Status!E:E,"LOW STOCK")</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>

</xml_diff>